<commit_message>
[add]: combined graphs and results are added
</commit_message>
<xml_diff>
--- a/CURRENT WORK/RESULT GRAPHS/OUR WORK GRAPHS/N=3 RESULT GRAPHS.xlsx
+++ b/CURRENT WORK/RESULT GRAPHS/OUR WORK GRAPHS/N=3 RESULT GRAPHS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\Final-Year-Project\CURRENT WORK\RESULT GRAPHS\OUR WORK GRAPHS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41C342D-6C5B-4A48-A79F-D670FF945EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB56476-0477-4A1B-8A61-935C9C4ACFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaCl2" sheetId="1" r:id="rId1"/>
@@ -5242,639 +5242,639 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="216"/>
                 <c:pt idx="1">
+                  <c:v>1.0690099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.87451E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3374199999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2256799999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4043499999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10764600000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.115548</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11946</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14311399999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.15495300000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>0.156919</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15622800000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.155999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15576999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15554200000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15531400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.155087</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.154861</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.15463499999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.15440999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.15418599999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.15396199999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.15373800000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.15351600000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.15329400000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.15285099999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.15263099999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.15241199999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.15219299999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.151975</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.15132399999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.150894</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.15068000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.15046699999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.15004200000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.14983099999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.14962</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.14941099999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.149201</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.14899299999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.148786</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.14857899999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.14816699999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.147759</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.14755599999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.14735400000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.14715300000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.146952</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.14675199999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.14655299999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14635500000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.14615700000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.14537600000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.14499000000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.14479900000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.14441799999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.144229</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.144041</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.14385400000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.14366799999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.143482</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.14329800000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
                   <c:v>0.14311399999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11946</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.10764600000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.115548</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.4043499999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.2256799999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.3374199999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.87451E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0690099999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.156919</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.15622800000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.155999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.15576999999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.15554200000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.15531400000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.155087</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.154861</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.15463499999999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.15440999999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.15418599999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.15396199999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.15373800000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.15351600000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.15329400000000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.15285099999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.15263099999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.15241199999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.15219299999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.151975</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.15132399999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.150894</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.15068000000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.15046699999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.15004200000000001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.14983099999999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.14962</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.14941099999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.149201</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.14899299999999999</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.148786</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.14857899999999999</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.14816699999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.147759</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.14755599999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.14735400000000001</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.14715300000000001</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.146952</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.14675199999999999</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.14655299999999999</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.14635500000000001</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.14615700000000001</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.14537600000000001</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.14499000000000001</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.14479900000000001</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.14441799999999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.144229</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.144041</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.14385400000000001</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.14366799999999999</c:v>
-                </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.143482</c:v>
+                  <c:v>0.142932</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.14329800000000001</c:v>
+                  <c:v>0.142569</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.14311399999999999</c:v>
+                  <c:v>0.14238899999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.142932</c:v>
+                  <c:v>0.14221</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.142569</c:v>
+                  <c:v>0.14203199999999999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.14238899999999999</c:v>
+                  <c:v>0.14185500000000001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.14221</c:v>
+                  <c:v>0.141678</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.14203199999999999</c:v>
+                  <c:v>0.14150299999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.14185500000000001</c:v>
+                  <c:v>0.14132900000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.141678</c:v>
+                  <c:v>0.141155</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.14150299999999999</c:v>
+                  <c:v>0.140983</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.14132900000000001</c:v>
+                  <c:v>0.14064099999999999</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.141155</c:v>
+                  <c:v>0.14030300000000001</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.140983</c:v>
+                  <c:v>0.14013600000000001</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.14064099999999999</c:v>
+                  <c:v>0.13963900000000001</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.14030300000000001</c:v>
+                  <c:v>0.13947599999999999</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.14013600000000001</c:v>
+                  <c:v>0.13931299999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.13963900000000001</c:v>
+                  <c:v>0.139152</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.13947599999999999</c:v>
+                  <c:v>0.13883200000000001</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.13931299999999999</c:v>
+                  <c:v>0.138517</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.139152</c:v>
+                  <c:v>0.13836000000000001</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.13883200000000001</c:v>
+                  <c:v>0.13820499999999999</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.138517</c:v>
+                  <c:v>0.13805100000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.13836000000000001</c:v>
+                  <c:v>0.13789799999999999</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.13820499999999999</c:v>
+                  <c:v>0.137297</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.13805100000000001</c:v>
+                  <c:v>0.13714899999999999</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.13789799999999999</c:v>
+                  <c:v>0.13700300000000001</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.137297</c:v>
+                  <c:v>0.13685700000000001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.13714899999999999</c:v>
+                  <c:v>0.136713</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.13700300000000001</c:v>
+                  <c:v>0.13657</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.13685700000000001</c:v>
+                  <c:v>0.13642799999999999</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.136713</c:v>
+                  <c:v>0.13628699999999999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.13657</c:v>
+                  <c:v>0.13600899999999999</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.13642799999999999</c:v>
+                  <c:v>0.13587099999999999</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.13628699999999999</c:v>
+                  <c:v>0.13573499999999999</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.13600899999999999</c:v>
+                  <c:v>0.135599</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.13587099999999999</c:v>
+                  <c:v>0.135465</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.13573499999999999</c:v>
+                  <c:v>0.13533300000000001</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.135599</c:v>
+                  <c:v>0.13520099999999999</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.135465</c:v>
+                  <c:v>0.13507</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.13533300000000001</c:v>
+                  <c:v>0.134686</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.13520099999999999</c:v>
+                  <c:v>0.13456000000000001</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.13507</c:v>
+                  <c:v>0.134436</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.134686</c:v>
+                  <c:v>0.13431199999999999</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.13456000000000001</c:v>
+                  <c:v>0.13419</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.134436</c:v>
+                  <c:v>0.13406899999999999</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.13431199999999999</c:v>
+                  <c:v>0.13394900000000001</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.13419</c:v>
+                  <c:v>0.13383100000000001</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.13406899999999999</c:v>
+                  <c:v>0.133714</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.13394900000000001</c:v>
+                  <c:v>0.13359799999999999</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.13383100000000001</c:v>
+                  <c:v>0.13348299999999999</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.133714</c:v>
+                  <c:v>0.13336999999999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.13359799999999999</c:v>
+                  <c:v>0.13325699999999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.13348299999999999</c:v>
+                  <c:v>0.13314599999999999</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.13336999999999999</c:v>
+                  <c:v>0.13303699999999999</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.13325699999999999</c:v>
+                  <c:v>0.13292799999999999</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.13314599999999999</c:v>
+                  <c:v>0.13282099999999999</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.13303699999999999</c:v>
+                  <c:v>0.13261100000000001</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.13292799999999999</c:v>
+                  <c:v>0.13240499999999999</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.13282099999999999</c:v>
+                  <c:v>0.13230500000000001</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.13261100000000001</c:v>
+                  <c:v>0.13220499999999999</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0.13240499999999999</c:v>
+                  <c:v>0.132107</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0.13230500000000001</c:v>
+                  <c:v>0.13201099999999999</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0.13220499999999999</c:v>
+                  <c:v>0.13182099999999999</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.132107</c:v>
+                  <c:v>0.13172900000000001</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0.13201099999999999</c:v>
+                  <c:v>0.131637</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0.13182099999999999</c:v>
+                  <c:v>0.131547</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0.13172900000000001</c:v>
+                  <c:v>0.13145799999999999</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0.131637</c:v>
+                  <c:v>0.13137099999999999</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0.131547</c:v>
+                  <c:v>0.13128500000000001</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.13145799999999999</c:v>
+                  <c:v>0.13120100000000001</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0.13137099999999999</c:v>
+                  <c:v>0.13111700000000001</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0.13128500000000001</c:v>
+                  <c:v>0.13103600000000001</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0.13120100000000001</c:v>
+                  <c:v>0.13095499999999999</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0.13111700000000001</c:v>
+                  <c:v>0.13087599999999999</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0.13103600000000001</c:v>
+                  <c:v>0.130722</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0.13095499999999999</c:v>
+                  <c:v>0.13064700000000001</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0.13087599999999999</c:v>
+                  <c:v>0.130574</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>0.130722</c:v>
+                  <c:v>0.13050200000000001</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>0.13064700000000001</c:v>
+                  <c:v>0.13036200000000001</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>0.130574</c:v>
+                  <c:v>0.13029499999999999</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>0.13050200000000001</c:v>
+                  <c:v>0.130163</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0.13036200000000001</c:v>
+                  <c:v>0.13009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0.13029499999999999</c:v>
+                  <c:v>0.13003799999999999</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0.130163</c:v>
+                  <c:v>0.12991900000000001</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>0.13009999999999999</c:v>
+                  <c:v>0.129861</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.13003799999999999</c:v>
+                  <c:v>0.129805</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>0.12991900000000001</c:v>
+                  <c:v>0.12975100000000001</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>0.129861</c:v>
+                  <c:v>0.12969800000000001</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>0.129805</c:v>
+                  <c:v>0.12964600000000001</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>0.12975100000000001</c:v>
+                  <c:v>0.12959599999999999</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0.12969800000000001</c:v>
+                  <c:v>0.129547</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0.12964600000000001</c:v>
+                  <c:v>0.1295</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>0.12959599999999999</c:v>
+                  <c:v>0.12945499999999999</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>0.129547</c:v>
+                  <c:v>0.129411</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>0.1295</c:v>
+                  <c:v>0.12928799999999999</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>0.12945499999999999</c:v>
+                  <c:v>0.12925</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>0.129411</c:v>
+                  <c:v>0.12917899999999999</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>0.12928799999999999</c:v>
+                  <c:v>0.12911400000000001</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0.12925</c:v>
+                  <c:v>0.129084</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>0.12917899999999999</c:v>
+                  <c:v>0.129056</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>0.12911400000000001</c:v>
+                  <c:v>0.129029</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>0.129084</c:v>
+                  <c:v>0.12900300000000001</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>0.129056</c:v>
+                  <c:v>0.12898000000000001</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>0.129029</c:v>
+                  <c:v>0.12895799999999999</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>0.12900300000000001</c:v>
+                  <c:v>0.128937</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>0.12898000000000001</c:v>
+                  <c:v>0.128918</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0.12895799999999999</c:v>
+                  <c:v>0.12890099999999999</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0.128937</c:v>
+                  <c:v>0.128885</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0.128918</c:v>
+                  <c:v>0.12887100000000001</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0.12890099999999999</c:v>
+                  <c:v>0.12883900000000001</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>0.128885</c:v>
+                  <c:v>0.128831</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0.12887100000000001</c:v>
+                  <c:v>0.128825</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0.12883900000000001</c:v>
+                  <c:v>0.12881899999999999</c:v>
                 </c:pt>
                 <c:pt idx="178">
+                  <c:v>0.12881799999999999</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.12881799999999999</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.12882099999999999</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.128825</c:v>
+                </c:pt>
+                <c:pt idx="182">
                   <c:v>0.128831</c:v>
                 </c:pt>
-                <c:pt idx="179">
-                  <c:v>0.128825</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>0.12881899999999999</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0.12881799999999999</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>0.12881799999999999</c:v>
-                </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.12882099999999999</c:v>
+                  <c:v>0.12884799999999999</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.128825</c:v>
+                  <c:v>0.128859</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>0.128831</c:v>
+                  <c:v>0.128886</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>0.12884799999999999</c:v>
+                  <c:v>0.12890199999999999</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>0.128859</c:v>
+                  <c:v>0.128939</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0.128886</c:v>
+                  <c:v>0.12896099999999999</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.12890199999999999</c:v>
+                  <c:v>0.12898399999999999</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>0.128939</c:v>
+                  <c:v>0.12900800000000001</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>0.12896099999999999</c:v>
+                  <c:v>0.12903500000000001</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0.12898399999999999</c:v>
+                  <c:v>0.12906300000000001</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0.12900800000000001</c:v>
+                  <c:v>0.12909300000000001</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.12903500000000001</c:v>
+                  <c:v>0.12912499999999999</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.12906300000000001</c:v>
+                  <c:v>0.129159</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.12909300000000001</c:v>
+                  <c:v>0.129194</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.12912499999999999</c:v>
+                  <c:v>0.12927</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>0.129159</c:v>
+                  <c:v>0.129354</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0.129194</c:v>
+                  <c:v>0.12939800000000001</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0.12927</c:v>
+                  <c:v>0.129444</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>0.129354</c:v>
+                  <c:v>0.129492</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>0.12939800000000001</c:v>
+                  <c:v>0.12954199999999999</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>0.129444</c:v>
+                  <c:v>0.12959399999999999</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>0.129492</c:v>
+                  <c:v>0.12964700000000001</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>0.12954199999999999</c:v>
+                  <c:v>0.12970300000000001</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>0.12959399999999999</c:v>
+                  <c:v>0.12975999999999999</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>0.12964700000000001</c:v>
+                  <c:v>0.12988</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>0.12970300000000001</c:v>
+                  <c:v>0.129942</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>0.12975999999999999</c:v>
+                  <c:v>0.13000700000000001</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>0.12988</c:v>
+                  <c:v>0.130074</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>0.129942</c:v>
+                  <c:v>0.13014200000000001</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>0.13000700000000001</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>0.130074</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>0.13014200000000001</c:v>
-                </c:pt>
-                <c:pt idx="215">
                   <c:v>0.13021199999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -5887,639 +5887,639 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="216"/>
                 <c:pt idx="1">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>257</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>258</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="18">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="20">
                   <c:v>261</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="22">
                   <c:v>263</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
                   <c:v>264</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
                   <c:v>265</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="25">
                   <c:v>266</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>253</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>255</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>257</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>258</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>261</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>263</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>264</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>265</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>266</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>268</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>269</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>270</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>271</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>272</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>275</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>277</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>278</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>279</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>281</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>282</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>283</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>284</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>285</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>286</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>287</c:v>
+                  <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>288</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>290</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>292</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>293</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>294</c:v>
+                  <c:v>297</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>295</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>296</c:v>
+                  <c:v>299</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>297</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>298</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>299</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>300</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>304</c:v>
+                  <c:v>309</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>306</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>307</c:v>
+                  <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>309</c:v>
+                  <c:v>312</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>310</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>311</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>312</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>313</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>314</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>315</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>316</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>317</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>319</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>320</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>321</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>322</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>323</c:v>
+                  <c:v>326</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>324</c:v>
+                  <c:v>327</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>325</c:v>
+                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>326</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>327</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>328</c:v>
+                  <c:v>333</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>330</c:v>
+                  <c:v>336</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>332</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>333</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>336</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>337</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>338</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>339</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>341</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>343</c:v>
+                  <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>344</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>345</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>346</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>347</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>351</c:v>
+                  <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>352</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>353</c:v>
+                  <c:v>356</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>354</c:v>
+                  <c:v>357</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>355</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>356</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>357</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>358</c:v>
+                  <c:v>362</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>360</c:v>
+                  <c:v>363</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>361</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>362</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>363</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>364</c:v>
+                  <c:v>367</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>365</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>366</c:v>
+                  <c:v>371</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>367</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>370</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>371</c:v>
+                  <c:v>374</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>372</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>373</c:v>
+                  <c:v>376</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>374</c:v>
+                  <c:v>377</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>375</c:v>
+                  <c:v>378</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>376</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>377</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>378</c:v>
+                  <c:v>381</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>379</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>380</c:v>
+                  <c:v>383</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>381</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>382</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>383</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>384</c:v>
+                  <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>385</c:v>
+                  <c:v>390</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>386</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>388</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>390</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>391</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>392</c:v>
+                  <c:v>396</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>393</c:v>
+                  <c:v>397</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>394</c:v>
+                  <c:v>398</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>396</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>397</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>398</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>399</c:v>
+                  <c:v>402</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>400</c:v>
+                  <c:v>403</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>401</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>402</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>403</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>404</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>405</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>406</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>407</c:v>
+                  <c:v>411</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>409</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>410</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>411</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>412</c:v>
+                  <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>414</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>415</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>417</c:v>
+                  <c:v>421</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>418</c:v>
+                  <c:v>422</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>419</c:v>
+                  <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>421</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>422</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>423</c:v>
+                  <c:v>426</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>424</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>425</c:v>
+                  <c:v>428</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>426</c:v>
+                  <c:v>429</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>427</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>428</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>429</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>430</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>431</c:v>
+                  <c:v>437</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>434</c:v>
+                  <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>435</c:v>
+                  <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>437</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>439</c:v>
+                  <c:v>442</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>440</c:v>
+                  <c:v>443</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>441</c:v>
+                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>442</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>443</c:v>
+                  <c:v>446</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>444</c:v>
+                  <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>445</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>446</c:v>
+                  <c:v>449</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>447</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>448</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>449</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>450</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>453</c:v>
+                  <c:v>457</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>454</c:v>
+                  <c:v>458</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>455</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>457</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>458</c:v>
+                  <c:v>461</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>459</c:v>
+                  <c:v>462</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>460</c:v>
+                  <c:v>464</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>461</c:v>
+                  <c:v>465</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>462</c:v>
+                  <c:v>467</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>464</c:v>
+                  <c:v>468</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>465</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>467</c:v>
+                  <c:v>471</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>468</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>470</c:v>
+                  <c:v>473</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>471</c:v>
+                  <c:v>474</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>472</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>473</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>474</c:v>
+                  <c:v>477</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>475</c:v>
+                  <c:v>478</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>476</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>477</c:v>
+                  <c:v>481</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>478</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>479</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>481</c:v>
+                  <c:v>485</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>483</c:v>
+                  <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>484</c:v>
+                  <c:v>487</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>485</c:v>
+                  <c:v>488</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>486</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>487</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>488</c:v>
+                  <c:v>491</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>489</c:v>
+                  <c:v>493</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>490</c:v>
+                  <c:v>494</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>491</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>493</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>494</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>495</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>496</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>497</c:v>
-                </c:pt>
-                <c:pt idx="215">
                   <c:v>498</c:v>
                 </c:pt>
               </c:numCache>
@@ -26418,10 +26418,10 @@
             <v>268.44208538099599</v>
           </cell>
           <cell r="D5">
-            <v>0.15495300000000001</v>
+            <v>1.0690099999999999E-2</v>
           </cell>
           <cell r="E5">
-            <v>257</v>
+            <v>267</v>
           </cell>
         </row>
         <row r="6">
@@ -26432,10 +26432,10 @@
             <v>267.91479389286201</v>
           </cell>
           <cell r="D6">
-            <v>0.14311399999999999</v>
+            <v>4.87451E-2</v>
           </cell>
           <cell r="E6">
-            <v>258</v>
+            <v>266</v>
           </cell>
         </row>
         <row r="7">
@@ -26446,10 +26446,10 @@
             <v>263.97715944664998</v>
           </cell>
           <cell r="D7">
-            <v>0.11946</v>
+            <v>5.3374199999999997E-2</v>
           </cell>
           <cell r="E7">
-            <v>260</v>
+            <v>265</v>
           </cell>
         </row>
         <row r="8">
@@ -26460,10 +26460,10 @@
             <v>260.064009513982</v>
           </cell>
           <cell r="D8">
-            <v>0.10764600000000001</v>
+            <v>7.2256799999999996E-2</v>
           </cell>
           <cell r="E8">
-            <v>261</v>
+            <v>264</v>
           </cell>
         </row>
         <row r="9">
@@ -26474,10 +26474,10 @@
             <v>254.423826929467</v>
           </cell>
           <cell r="D9">
-            <v>0.115548</v>
+            <v>8.4043499999999993E-2</v>
           </cell>
           <cell r="E9">
-            <v>262</v>
+            <v>263</v>
           </cell>
         </row>
         <row r="10">
@@ -26488,10 +26488,10 @@
             <v>252.75800556148201</v>
           </cell>
           <cell r="D10">
-            <v>8.4043499999999993E-2</v>
+            <v>0.10764600000000001</v>
           </cell>
           <cell r="E10">
-            <v>263</v>
+            <v>261</v>
           </cell>
         </row>
         <row r="11">
@@ -26502,10 +26502,10 @@
             <v>255.604330261109</v>
           </cell>
           <cell r="D11">
-            <v>7.2256799999999996E-2</v>
+            <v>0.115548</v>
           </cell>
           <cell r="E11">
-            <v>264</v>
+            <v>262</v>
           </cell>
         </row>
         <row r="12">
@@ -26516,10 +26516,10 @@
             <v>256.74023680022299</v>
           </cell>
           <cell r="D12">
-            <v>5.3374199999999997E-2</v>
+            <v>0.11946</v>
           </cell>
           <cell r="E12">
-            <v>265</v>
+            <v>260</v>
           </cell>
         </row>
         <row r="13">
@@ -26530,10 +26530,10 @@
             <v>260.72596582661401</v>
           </cell>
           <cell r="D13">
-            <v>4.87451E-2</v>
+            <v>0.14311399999999999</v>
           </cell>
           <cell r="E13">
-            <v>266</v>
+            <v>258</v>
           </cell>
         </row>
         <row r="14">
@@ -26544,10 +26544,10 @@
             <v>263.56791829167997</v>
           </cell>
           <cell r="D14">
-            <v>1.0690099999999999E-2</v>
+            <v>0.15495300000000001</v>
           </cell>
           <cell r="E14">
-            <v>267</v>
+            <v>257</v>
           </cell>
         </row>
         <row r="15">
@@ -26557,6 +26557,12 @@
           <cell r="B15">
             <v>268.12028891725902</v>
           </cell>
+          <cell r="D15">
+            <v>0.156919</v>
+          </cell>
+          <cell r="E15">
+            <v>250</v>
+          </cell>
         </row>
         <row r="16">
           <cell r="A16">
@@ -26565,6 +26571,12 @@
           <cell r="B16">
             <v>272.10252015600099</v>
           </cell>
+          <cell r="D16">
+            <v>0.15622800000000001</v>
+          </cell>
+          <cell r="E16">
+            <v>253</v>
+          </cell>
         </row>
         <row r="17">
           <cell r="A17">
@@ -26573,6 +26585,12 @@
           <cell r="B17">
             <v>281.77127966561102</v>
           </cell>
+          <cell r="D17">
+            <v>0.155999</v>
+          </cell>
+          <cell r="E17">
+            <v>254</v>
+          </cell>
         </row>
         <row r="18">
           <cell r="A18">
@@ -26582,10 +26600,10 @@
             <v>289.16647720316899</v>
           </cell>
           <cell r="D18">
-            <v>0.156919</v>
+            <v>0.15576999999999999</v>
           </cell>
           <cell r="E18">
-            <v>250</v>
+            <v>255</v>
           </cell>
         </row>
         <row r="19">
@@ -26596,10 +26614,10 @@
             <v>295.992409800801</v>
           </cell>
           <cell r="D19">
-            <v>0.15622800000000001</v>
+            <v>0.15554200000000001</v>
           </cell>
           <cell r="E19">
-            <v>253</v>
+            <v>256</v>
           </cell>
         </row>
         <row r="20">
@@ -26610,10 +26628,10 @@
             <v>303.38848178527002</v>
           </cell>
           <cell r="D20">
-            <v>0.155999</v>
+            <v>0.15531400000000001</v>
           </cell>
           <cell r="E20">
-            <v>254</v>
+            <v>257</v>
           </cell>
         </row>
         <row r="21">
@@ -26624,10 +26642,10 @@
             <v>307.37071302401199</v>
           </cell>
           <cell r="D21">
-            <v>0.15576999999999999</v>
+            <v>0.155087</v>
           </cell>
           <cell r="E21">
-            <v>255</v>
+            <v>258</v>
           </cell>
         </row>
         <row r="22">
@@ -26638,10 +26656,10 @@
             <v>313.63000402245501</v>
           </cell>
           <cell r="D22">
-            <v>0.15554200000000001</v>
+            <v>0.154861</v>
           </cell>
           <cell r="E22">
-            <v>256</v>
+            <v>259</v>
           </cell>
         </row>
         <row r="23">
@@ -26652,10 +26670,10 @@
             <v>319.89104391472398</v>
           </cell>
           <cell r="D23">
-            <v>0.15531400000000001</v>
+            <v>0.15463499999999999</v>
           </cell>
           <cell r="E23">
-            <v>257</v>
+            <v>260</v>
           </cell>
         </row>
         <row r="24">
@@ -26666,10 +26684,10 @@
             <v>323.87152625964001</v>
           </cell>
           <cell r="D24">
-            <v>0.155087</v>
+            <v>0.15440999999999999</v>
           </cell>
           <cell r="E24">
-            <v>258</v>
+            <v>261</v>
           </cell>
         </row>
         <row r="25">
@@ -26680,10 +26698,10 @@
             <v>327.28536700536898</v>
           </cell>
           <cell r="D25">
-            <v>0.154861</v>
+            <v>0.15418599999999999</v>
           </cell>
           <cell r="E25">
-            <v>259</v>
+            <v>262</v>
           </cell>
         </row>
         <row r="26">
@@ -26694,10 +26712,10 @@
             <v>339.23118627468102</v>
           </cell>
           <cell r="D26">
-            <v>0.15463499999999999</v>
+            <v>0.15396199999999999</v>
           </cell>
           <cell r="E26">
-            <v>260</v>
+            <v>263</v>
           </cell>
         </row>
         <row r="27">
@@ -26708,10 +26726,10 @@
             <v>348.90694135959001</v>
           </cell>
           <cell r="D27">
-            <v>0.15440999999999999</v>
+            <v>0.15373800000000001</v>
           </cell>
           <cell r="E27">
-            <v>261</v>
+            <v>264</v>
           </cell>
         </row>
         <row r="28">
@@ -26722,10 +26740,10 @@
             <v>350.04109900487902</v>
           </cell>
           <cell r="D28">
-            <v>0.15418599999999999</v>
+            <v>0.15351600000000001</v>
           </cell>
           <cell r="E28">
-            <v>262</v>
+            <v>265</v>
           </cell>
         </row>
         <row r="29">
@@ -26736,10 +26754,10 @@
             <v>365.41125238286702</v>
           </cell>
           <cell r="D29">
-            <v>0.15396199999999999</v>
+            <v>0.15329400000000001</v>
           </cell>
           <cell r="E29">
-            <v>263</v>
+            <v>266</v>
           </cell>
         </row>
         <row r="30">
@@ -26750,10 +26768,10 @@
             <v>368.82334423477101</v>
           </cell>
           <cell r="D30">
-            <v>0.15373800000000001</v>
+            <v>0.15285099999999999</v>
           </cell>
           <cell r="E30">
-            <v>264</v>
+            <v>268</v>
           </cell>
         </row>
         <row r="31">
@@ -26764,10 +26782,10 @@
             <v>372.806449920425</v>
           </cell>
           <cell r="D31">
-            <v>0.15351600000000001</v>
+            <v>0.15263099999999999</v>
           </cell>
           <cell r="E31">
-            <v>265</v>
+            <v>269</v>
           </cell>
         </row>
         <row r="32">
@@ -26778,10 +26796,10 @@
             <v>377.36056943982902</v>
           </cell>
           <cell r="D32">
-            <v>0.15329400000000001</v>
+            <v>0.15241199999999999</v>
           </cell>
           <cell r="E32">
-            <v>266</v>
+            <v>270</v>
           </cell>
         </row>
         <row r="33">
@@ -26792,10 +26810,10 @@
             <v>418.33452841078002</v>
           </cell>
           <cell r="D33">
-            <v>0.15285099999999999</v>
+            <v>0.15219299999999999</v>
           </cell>
           <cell r="E33">
-            <v>268</v>
+            <v>271</v>
           </cell>
         </row>
         <row r="34">
@@ -26806,10 +26824,10 @@
             <v>461.02590111754301</v>
           </cell>
           <cell r="D34">
-            <v>0.15263099999999999</v>
+            <v>0.151975</v>
           </cell>
           <cell r="E34">
-            <v>269</v>
+            <v>272</v>
           </cell>
         </row>
         <row r="35">
@@ -26820,1481 +26838,1457 @@
             <v>488.35324157470399</v>
           </cell>
           <cell r="D35">
-            <v>0.15241199999999999</v>
+            <v>0.15132399999999999</v>
           </cell>
           <cell r="E35">
-            <v>270</v>
+            <v>275</v>
           </cell>
         </row>
         <row r="36">
           <cell r="D36">
-            <v>0.15219299999999999</v>
+            <v>0.150894</v>
           </cell>
           <cell r="E36">
-            <v>271</v>
+            <v>277</v>
           </cell>
         </row>
         <row r="37">
           <cell r="D37">
-            <v>0.151975</v>
+            <v>0.15068000000000001</v>
           </cell>
           <cell r="E37">
-            <v>272</v>
+            <v>278</v>
           </cell>
         </row>
         <row r="38">
           <cell r="D38">
-            <v>0.15132399999999999</v>
+            <v>0.15046699999999999</v>
           </cell>
           <cell r="E38">
-            <v>275</v>
+            <v>279</v>
           </cell>
         </row>
         <row r="39">
           <cell r="D39">
-            <v>0.150894</v>
+            <v>0.15004200000000001</v>
           </cell>
           <cell r="E39">
-            <v>277</v>
+            <v>281</v>
           </cell>
         </row>
         <row r="40">
           <cell r="D40">
-            <v>0.15068000000000001</v>
+            <v>0.14983099999999999</v>
           </cell>
           <cell r="E40">
-            <v>278</v>
+            <v>282</v>
           </cell>
         </row>
         <row r="41">
           <cell r="D41">
-            <v>0.15046699999999999</v>
+            <v>0.14962</v>
           </cell>
           <cell r="E41">
-            <v>279</v>
+            <v>283</v>
           </cell>
         </row>
         <row r="42">
           <cell r="D42">
-            <v>0.15004200000000001</v>
+            <v>0.14941099999999999</v>
           </cell>
           <cell r="E42">
-            <v>281</v>
+            <v>284</v>
           </cell>
         </row>
         <row r="43">
           <cell r="D43">
-            <v>0.14983099999999999</v>
+            <v>0.149201</v>
           </cell>
           <cell r="E43">
-            <v>282</v>
+            <v>285</v>
           </cell>
         </row>
         <row r="44">
           <cell r="D44">
-            <v>0.14962</v>
+            <v>0.14899299999999999</v>
           </cell>
           <cell r="E44">
-            <v>283</v>
+            <v>286</v>
           </cell>
         </row>
         <row r="45">
           <cell r="D45">
-            <v>0.14941099999999999</v>
+            <v>0.148786</v>
           </cell>
           <cell r="E45">
-            <v>284</v>
+            <v>287</v>
           </cell>
         </row>
         <row r="46">
           <cell r="D46">
-            <v>0.149201</v>
+            <v>0.14857899999999999</v>
           </cell>
           <cell r="E46">
-            <v>285</v>
+            <v>288</v>
           </cell>
         </row>
         <row r="47">
           <cell r="D47">
-            <v>0.14899299999999999</v>
+            <v>0.14816699999999999</v>
           </cell>
           <cell r="E47">
-            <v>286</v>
+            <v>290</v>
           </cell>
         </row>
         <row r="48">
           <cell r="D48">
-            <v>0.148786</v>
+            <v>0.147759</v>
           </cell>
           <cell r="E48">
-            <v>287</v>
+            <v>292</v>
           </cell>
         </row>
         <row r="49">
           <cell r="D49">
-            <v>0.14857899999999999</v>
+            <v>0.14755599999999999</v>
           </cell>
           <cell r="E49">
-            <v>288</v>
+            <v>293</v>
           </cell>
         </row>
         <row r="50">
           <cell r="D50">
-            <v>0.14816699999999999</v>
+            <v>0.14735400000000001</v>
           </cell>
           <cell r="E50">
-            <v>290</v>
+            <v>294</v>
           </cell>
         </row>
         <row r="51">
           <cell r="D51">
-            <v>0.147759</v>
+            <v>0.14715300000000001</v>
           </cell>
           <cell r="E51">
-            <v>292</v>
+            <v>295</v>
           </cell>
         </row>
         <row r="52">
           <cell r="D52">
-            <v>0.14755599999999999</v>
+            <v>0.146952</v>
           </cell>
           <cell r="E52">
-            <v>293</v>
+            <v>296</v>
           </cell>
         </row>
         <row r="53">
           <cell r="D53">
-            <v>0.14735400000000001</v>
+            <v>0.14675199999999999</v>
           </cell>
           <cell r="E53">
-            <v>294</v>
+            <v>297</v>
           </cell>
         </row>
         <row r="54">
           <cell r="D54">
-            <v>0.14715300000000001</v>
+            <v>0.14655299999999999</v>
           </cell>
           <cell r="E54">
-            <v>295</v>
+            <v>298</v>
           </cell>
         </row>
         <row r="55">
           <cell r="D55">
-            <v>0.146952</v>
+            <v>0.14635500000000001</v>
           </cell>
           <cell r="E55">
-            <v>296</v>
+            <v>299</v>
           </cell>
         </row>
         <row r="56">
           <cell r="D56">
-            <v>0.14675199999999999</v>
+            <v>0.14615700000000001</v>
           </cell>
           <cell r="E56">
-            <v>297</v>
+            <v>300</v>
           </cell>
         </row>
         <row r="57">
           <cell r="D57">
-            <v>0.14655299999999999</v>
+            <v>0.14537600000000001</v>
           </cell>
           <cell r="E57">
-            <v>298</v>
+            <v>304</v>
           </cell>
         </row>
         <row r="58">
           <cell r="D58">
-            <v>0.14635500000000001</v>
+            <v>0.14499000000000001</v>
           </cell>
           <cell r="E58">
-            <v>299</v>
+            <v>306</v>
           </cell>
         </row>
         <row r="59">
           <cell r="D59">
-            <v>0.14615700000000001</v>
+            <v>0.14479900000000001</v>
           </cell>
           <cell r="E59">
-            <v>300</v>
+            <v>307</v>
           </cell>
         </row>
         <row r="60">
           <cell r="D60">
-            <v>0.14537600000000001</v>
+            <v>0.14441799999999999</v>
           </cell>
           <cell r="E60">
-            <v>304</v>
+            <v>309</v>
           </cell>
         </row>
         <row r="61">
           <cell r="D61">
-            <v>0.14499000000000001</v>
+            <v>0.144229</v>
           </cell>
           <cell r="E61">
-            <v>306</v>
+            <v>310</v>
           </cell>
         </row>
         <row r="62">
           <cell r="D62">
-            <v>0.14479900000000001</v>
+            <v>0.144041</v>
           </cell>
           <cell r="E62">
-            <v>307</v>
+            <v>311</v>
           </cell>
         </row>
         <row r="63">
           <cell r="D63">
-            <v>0.14441799999999999</v>
+            <v>0.14385400000000001</v>
           </cell>
           <cell r="E63">
-            <v>309</v>
+            <v>312</v>
           </cell>
         </row>
         <row r="64">
           <cell r="D64">
-            <v>0.144229</v>
+            <v>0.14366799999999999</v>
           </cell>
           <cell r="E64">
-            <v>310</v>
+            <v>313</v>
           </cell>
         </row>
         <row r="65">
           <cell r="D65">
-            <v>0.144041</v>
+            <v>0.143482</v>
           </cell>
           <cell r="E65">
-            <v>311</v>
+            <v>314</v>
           </cell>
         </row>
         <row r="66">
           <cell r="D66">
-            <v>0.14385400000000001</v>
+            <v>0.14329800000000001</v>
           </cell>
           <cell r="E66">
-            <v>312</v>
+            <v>315</v>
           </cell>
         </row>
         <row r="67">
           <cell r="D67">
-            <v>0.14366799999999999</v>
+            <v>0.14311399999999999</v>
           </cell>
           <cell r="E67">
-            <v>313</v>
+            <v>316</v>
           </cell>
         </row>
         <row r="68">
           <cell r="D68">
-            <v>0.143482</v>
+            <v>0.142932</v>
           </cell>
           <cell r="E68">
-            <v>314</v>
+            <v>317</v>
           </cell>
         </row>
         <row r="69">
           <cell r="D69">
-            <v>0.14329800000000001</v>
+            <v>0.142569</v>
           </cell>
           <cell r="E69">
-            <v>315</v>
+            <v>319</v>
           </cell>
         </row>
         <row r="70">
           <cell r="D70">
-            <v>0.14311399999999999</v>
+            <v>0.14238899999999999</v>
           </cell>
           <cell r="E70">
-            <v>316</v>
+            <v>320</v>
           </cell>
         </row>
         <row r="71">
           <cell r="D71">
-            <v>0.142932</v>
+            <v>0.14221</v>
           </cell>
           <cell r="E71">
-            <v>317</v>
+            <v>321</v>
           </cell>
         </row>
         <row r="72">
           <cell r="D72">
-            <v>0.142569</v>
+            <v>0.14203199999999999</v>
           </cell>
           <cell r="E72">
-            <v>319</v>
+            <v>322</v>
           </cell>
         </row>
         <row r="73">
           <cell r="D73">
-            <v>0.14238899999999999</v>
+            <v>0.14185500000000001</v>
           </cell>
           <cell r="E73">
-            <v>320</v>
+            <v>323</v>
           </cell>
         </row>
         <row r="74">
           <cell r="D74">
-            <v>0.14221</v>
+            <v>0.141678</v>
           </cell>
           <cell r="E74">
-            <v>321</v>
+            <v>324</v>
           </cell>
         </row>
         <row r="75">
           <cell r="D75">
-            <v>0.14203199999999999</v>
+            <v>0.14150299999999999</v>
           </cell>
           <cell r="E75">
-            <v>322</v>
+            <v>325</v>
           </cell>
         </row>
         <row r="76">
           <cell r="D76">
-            <v>0.14185500000000001</v>
+            <v>0.14132900000000001</v>
           </cell>
           <cell r="E76">
-            <v>323</v>
+            <v>326</v>
           </cell>
         </row>
         <row r="77">
           <cell r="D77">
-            <v>0.141678</v>
+            <v>0.141155</v>
           </cell>
           <cell r="E77">
-            <v>324</v>
+            <v>327</v>
           </cell>
         </row>
         <row r="78">
           <cell r="D78">
-            <v>0.14150299999999999</v>
+            <v>0.140983</v>
           </cell>
           <cell r="E78">
-            <v>325</v>
+            <v>328</v>
           </cell>
         </row>
         <row r="79">
           <cell r="D79">
-            <v>0.14132900000000001</v>
+            <v>0.14064099999999999</v>
           </cell>
           <cell r="E79">
-            <v>326</v>
+            <v>330</v>
           </cell>
         </row>
         <row r="80">
           <cell r="D80">
-            <v>0.141155</v>
+            <v>0.14030300000000001</v>
           </cell>
           <cell r="E80">
-            <v>327</v>
+            <v>332</v>
           </cell>
         </row>
         <row r="81">
           <cell r="D81">
-            <v>0.140983</v>
+            <v>0.14013600000000001</v>
           </cell>
           <cell r="E81">
-            <v>328</v>
+            <v>333</v>
           </cell>
         </row>
         <row r="82">
           <cell r="D82">
-            <v>0.14064099999999999</v>
+            <v>0.13963900000000001</v>
           </cell>
           <cell r="E82">
-            <v>330</v>
+            <v>336</v>
           </cell>
         </row>
         <row r="83">
           <cell r="D83">
-            <v>0.14030300000000001</v>
+            <v>0.13947599999999999</v>
           </cell>
           <cell r="E83">
-            <v>332</v>
+            <v>337</v>
           </cell>
         </row>
         <row r="84">
           <cell r="D84">
-            <v>0.14013600000000001</v>
+            <v>0.13931299999999999</v>
           </cell>
           <cell r="E84">
-            <v>333</v>
+            <v>338</v>
           </cell>
         </row>
         <row r="85">
           <cell r="D85">
-            <v>0.13963900000000001</v>
+            <v>0.139152</v>
           </cell>
           <cell r="E85">
-            <v>336</v>
+            <v>339</v>
           </cell>
         </row>
         <row r="86">
           <cell r="D86">
-            <v>0.13947599999999999</v>
+            <v>0.13883200000000001</v>
           </cell>
           <cell r="E86">
-            <v>337</v>
+            <v>341</v>
           </cell>
         </row>
         <row r="87">
           <cell r="D87">
-            <v>0.13931299999999999</v>
+            <v>0.138517</v>
           </cell>
           <cell r="E87">
-            <v>338</v>
+            <v>343</v>
           </cell>
         </row>
         <row r="88">
           <cell r="D88">
-            <v>0.139152</v>
+            <v>0.13836000000000001</v>
           </cell>
           <cell r="E88">
-            <v>339</v>
+            <v>344</v>
           </cell>
         </row>
         <row r="89">
           <cell r="D89">
-            <v>0.13883200000000001</v>
+            <v>0.13820499999999999</v>
           </cell>
           <cell r="E89">
-            <v>341</v>
+            <v>345</v>
           </cell>
         </row>
         <row r="90">
           <cell r="D90">
-            <v>0.138517</v>
+            <v>0.13805100000000001</v>
           </cell>
           <cell r="E90">
-            <v>343</v>
+            <v>346</v>
           </cell>
         </row>
         <row r="91">
           <cell r="D91">
-            <v>0.13836000000000001</v>
+            <v>0.13789799999999999</v>
           </cell>
           <cell r="E91">
-            <v>344</v>
+            <v>347</v>
           </cell>
         </row>
         <row r="92">
           <cell r="D92">
-            <v>0.13820499999999999</v>
+            <v>0.137297</v>
           </cell>
           <cell r="E92">
-            <v>345</v>
+            <v>351</v>
           </cell>
         </row>
         <row r="93">
           <cell r="D93">
-            <v>0.13805100000000001</v>
+            <v>0.13714899999999999</v>
           </cell>
           <cell r="E93">
-            <v>346</v>
+            <v>352</v>
           </cell>
         </row>
         <row r="94">
           <cell r="D94">
-            <v>0.13789799999999999</v>
+            <v>0.13700300000000001</v>
           </cell>
           <cell r="E94">
-            <v>347</v>
+            <v>353</v>
           </cell>
         </row>
         <row r="95">
           <cell r="D95">
-            <v>0.137297</v>
+            <v>0.13685700000000001</v>
           </cell>
           <cell r="E95">
-            <v>351</v>
+            <v>354</v>
           </cell>
         </row>
         <row r="96">
           <cell r="D96">
-            <v>0.13714899999999999</v>
+            <v>0.136713</v>
           </cell>
           <cell r="E96">
-            <v>352</v>
+            <v>355</v>
           </cell>
         </row>
         <row r="97">
           <cell r="D97">
-            <v>0.13700300000000001</v>
+            <v>0.13657</v>
           </cell>
           <cell r="E97">
-            <v>353</v>
+            <v>356</v>
           </cell>
         </row>
         <row r="98">
           <cell r="D98">
-            <v>0.13685700000000001</v>
+            <v>0.13642799999999999</v>
           </cell>
           <cell r="E98">
-            <v>354</v>
+            <v>357</v>
           </cell>
         </row>
         <row r="99">
           <cell r="D99">
-            <v>0.136713</v>
+            <v>0.13628699999999999</v>
           </cell>
           <cell r="E99">
-            <v>355</v>
+            <v>358</v>
           </cell>
         </row>
         <row r="100">
           <cell r="D100">
-            <v>0.13657</v>
+            <v>0.13600899999999999</v>
           </cell>
           <cell r="E100">
-            <v>356</v>
+            <v>360</v>
           </cell>
         </row>
         <row r="101">
           <cell r="D101">
-            <v>0.13642799999999999</v>
+            <v>0.13587099999999999</v>
           </cell>
           <cell r="E101">
-            <v>357</v>
+            <v>361</v>
           </cell>
         </row>
         <row r="102">
           <cell r="D102">
-            <v>0.13628699999999999</v>
+            <v>0.13573499999999999</v>
           </cell>
           <cell r="E102">
-            <v>358</v>
+            <v>362</v>
           </cell>
         </row>
         <row r="103">
           <cell r="D103">
-            <v>0.13600899999999999</v>
+            <v>0.135599</v>
           </cell>
           <cell r="E103">
-            <v>360</v>
+            <v>363</v>
           </cell>
         </row>
         <row r="104">
           <cell r="D104">
-            <v>0.13587099999999999</v>
+            <v>0.135465</v>
           </cell>
           <cell r="E104">
-            <v>361</v>
+            <v>364</v>
           </cell>
         </row>
         <row r="105">
           <cell r="D105">
-            <v>0.13573499999999999</v>
+            <v>0.13533300000000001</v>
           </cell>
           <cell r="E105">
-            <v>362</v>
+            <v>365</v>
           </cell>
         </row>
         <row r="106">
           <cell r="D106">
-            <v>0.135599</v>
+            <v>0.13520099999999999</v>
           </cell>
           <cell r="E106">
-            <v>363</v>
+            <v>366</v>
           </cell>
         </row>
         <row r="107">
           <cell r="D107">
-            <v>0.135465</v>
+            <v>0.13507</v>
           </cell>
           <cell r="E107">
-            <v>364</v>
+            <v>367</v>
           </cell>
         </row>
         <row r="108">
           <cell r="D108">
-            <v>0.13533300000000001</v>
+            <v>0.134686</v>
           </cell>
           <cell r="E108">
-            <v>365</v>
+            <v>370</v>
           </cell>
         </row>
         <row r="109">
           <cell r="D109">
-            <v>0.13520099999999999</v>
+            <v>0.13456000000000001</v>
           </cell>
           <cell r="E109">
-            <v>366</v>
+            <v>371</v>
           </cell>
         </row>
         <row r="110">
           <cell r="D110">
-            <v>0.13507</v>
+            <v>0.134436</v>
           </cell>
           <cell r="E110">
-            <v>367</v>
+            <v>372</v>
           </cell>
         </row>
         <row r="111">
           <cell r="D111">
-            <v>0.134686</v>
+            <v>0.13431199999999999</v>
           </cell>
           <cell r="E111">
-            <v>370</v>
+            <v>373</v>
           </cell>
         </row>
         <row r="112">
           <cell r="D112">
-            <v>0.13456000000000001</v>
+            <v>0.13419</v>
           </cell>
           <cell r="E112">
-            <v>371</v>
+            <v>374</v>
           </cell>
         </row>
         <row r="113">
           <cell r="D113">
-            <v>0.134436</v>
+            <v>0.13406899999999999</v>
           </cell>
           <cell r="E113">
-            <v>372</v>
+            <v>375</v>
           </cell>
         </row>
         <row r="114">
           <cell r="D114">
-            <v>0.13431199999999999</v>
+            <v>0.13394900000000001</v>
           </cell>
           <cell r="E114">
-            <v>373</v>
+            <v>376</v>
           </cell>
         </row>
         <row r="115">
           <cell r="D115">
-            <v>0.13419</v>
+            <v>0.13383100000000001</v>
           </cell>
           <cell r="E115">
-            <v>374</v>
+            <v>377</v>
           </cell>
         </row>
         <row r="116">
           <cell r="D116">
-            <v>0.13406899999999999</v>
+            <v>0.133714</v>
           </cell>
           <cell r="E116">
-            <v>375</v>
+            <v>378</v>
           </cell>
         </row>
         <row r="117">
           <cell r="D117">
-            <v>0.13394900000000001</v>
+            <v>0.13359799999999999</v>
           </cell>
           <cell r="E117">
-            <v>376</v>
+            <v>379</v>
           </cell>
         </row>
         <row r="118">
           <cell r="D118">
-            <v>0.13383100000000001</v>
+            <v>0.13348299999999999</v>
           </cell>
           <cell r="E118">
-            <v>377</v>
+            <v>380</v>
           </cell>
         </row>
         <row r="119">
           <cell r="D119">
-            <v>0.133714</v>
+            <v>0.13336999999999999</v>
           </cell>
           <cell r="E119">
-            <v>378</v>
+            <v>381</v>
           </cell>
         </row>
         <row r="120">
           <cell r="D120">
-            <v>0.13359799999999999</v>
+            <v>0.13325699999999999</v>
           </cell>
           <cell r="E120">
-            <v>379</v>
+            <v>382</v>
           </cell>
         </row>
         <row r="121">
           <cell r="D121">
-            <v>0.13348299999999999</v>
+            <v>0.13314599999999999</v>
           </cell>
           <cell r="E121">
-            <v>380</v>
+            <v>383</v>
           </cell>
         </row>
         <row r="122">
           <cell r="D122">
-            <v>0.13336999999999999</v>
+            <v>0.13303699999999999</v>
           </cell>
           <cell r="E122">
-            <v>381</v>
+            <v>384</v>
           </cell>
         </row>
         <row r="123">
           <cell r="D123">
-            <v>0.13325699999999999</v>
+            <v>0.13292799999999999</v>
           </cell>
           <cell r="E123">
-            <v>382</v>
+            <v>385</v>
           </cell>
         </row>
         <row r="124">
           <cell r="D124">
-            <v>0.13314599999999999</v>
+            <v>0.13282099999999999</v>
           </cell>
           <cell r="E124">
-            <v>383</v>
+            <v>386</v>
           </cell>
         </row>
         <row r="125">
           <cell r="D125">
-            <v>0.13303699999999999</v>
+            <v>0.13261100000000001</v>
           </cell>
           <cell r="E125">
-            <v>384</v>
+            <v>388</v>
           </cell>
         </row>
         <row r="126">
           <cell r="D126">
-            <v>0.13292799999999999</v>
+            <v>0.13240499999999999</v>
           </cell>
           <cell r="E126">
-            <v>385</v>
+            <v>390</v>
           </cell>
         </row>
         <row r="127">
           <cell r="D127">
-            <v>0.13282099999999999</v>
+            <v>0.13230500000000001</v>
           </cell>
           <cell r="E127">
-            <v>386</v>
+            <v>391</v>
           </cell>
         </row>
         <row r="128">
           <cell r="D128">
-            <v>0.13261100000000001</v>
+            <v>0.13220499999999999</v>
           </cell>
           <cell r="E128">
-            <v>388</v>
+            <v>392</v>
           </cell>
         </row>
         <row r="129">
           <cell r="D129">
-            <v>0.13240499999999999</v>
+            <v>0.132107</v>
           </cell>
           <cell r="E129">
-            <v>390</v>
+            <v>393</v>
           </cell>
         </row>
         <row r="130">
           <cell r="D130">
-            <v>0.13230500000000001</v>
+            <v>0.13201099999999999</v>
           </cell>
           <cell r="E130">
-            <v>391</v>
+            <v>394</v>
           </cell>
         </row>
         <row r="131">
           <cell r="D131">
-            <v>0.13220499999999999</v>
+            <v>0.13182099999999999</v>
           </cell>
           <cell r="E131">
-            <v>392</v>
+            <v>396</v>
           </cell>
         </row>
         <row r="132">
           <cell r="D132">
-            <v>0.132107</v>
+            <v>0.13172900000000001</v>
           </cell>
           <cell r="E132">
-            <v>393</v>
+            <v>397</v>
           </cell>
         </row>
         <row r="133">
           <cell r="D133">
-            <v>0.13201099999999999</v>
+            <v>0.131637</v>
           </cell>
           <cell r="E133">
-            <v>394</v>
+            <v>398</v>
           </cell>
         </row>
         <row r="134">
           <cell r="D134">
-            <v>0.13182099999999999</v>
+            <v>0.131547</v>
           </cell>
           <cell r="E134">
-            <v>396</v>
+            <v>399</v>
           </cell>
         </row>
         <row r="135">
           <cell r="D135">
-            <v>0.13172900000000001</v>
+            <v>0.13145799999999999</v>
           </cell>
           <cell r="E135">
-            <v>397</v>
+            <v>400</v>
           </cell>
         </row>
         <row r="136">
           <cell r="D136">
-            <v>0.131637</v>
+            <v>0.13137099999999999</v>
           </cell>
           <cell r="E136">
-            <v>398</v>
+            <v>401</v>
           </cell>
         </row>
         <row r="137">
           <cell r="D137">
-            <v>0.131547</v>
+            <v>0.13128500000000001</v>
           </cell>
           <cell r="E137">
-            <v>399</v>
+            <v>402</v>
           </cell>
         </row>
         <row r="138">
           <cell r="D138">
-            <v>0.13145799999999999</v>
+            <v>0.13120100000000001</v>
           </cell>
           <cell r="E138">
-            <v>400</v>
+            <v>403</v>
           </cell>
         </row>
         <row r="139">
           <cell r="D139">
-            <v>0.13137099999999999</v>
+            <v>0.13111700000000001</v>
           </cell>
           <cell r="E139">
-            <v>401</v>
+            <v>404</v>
           </cell>
         </row>
         <row r="140">
           <cell r="D140">
-            <v>0.13128500000000001</v>
+            <v>0.13103600000000001</v>
           </cell>
           <cell r="E140">
-            <v>402</v>
+            <v>405</v>
           </cell>
         </row>
         <row r="141">
           <cell r="D141">
-            <v>0.13120100000000001</v>
+            <v>0.13095499999999999</v>
           </cell>
           <cell r="E141">
-            <v>403</v>
+            <v>406</v>
           </cell>
         </row>
         <row r="142">
           <cell r="D142">
-            <v>0.13111700000000001</v>
+            <v>0.13087599999999999</v>
           </cell>
           <cell r="E142">
-            <v>404</v>
+            <v>407</v>
           </cell>
         </row>
         <row r="143">
           <cell r="D143">
-            <v>0.13103600000000001</v>
+            <v>0.130722</v>
           </cell>
           <cell r="E143">
-            <v>405</v>
+            <v>409</v>
           </cell>
         </row>
         <row r="144">
           <cell r="D144">
-            <v>0.13095499999999999</v>
+            <v>0.13064700000000001</v>
           </cell>
           <cell r="E144">
-            <v>406</v>
+            <v>410</v>
           </cell>
         </row>
         <row r="145">
           <cell r="D145">
-            <v>0.13087599999999999</v>
+            <v>0.130574</v>
           </cell>
           <cell r="E145">
-            <v>407</v>
+            <v>411</v>
           </cell>
         </row>
         <row r="146">
           <cell r="D146">
-            <v>0.130722</v>
+            <v>0.13050200000000001</v>
           </cell>
           <cell r="E146">
-            <v>409</v>
+            <v>412</v>
           </cell>
         </row>
         <row r="147">
           <cell r="D147">
-            <v>0.13064700000000001</v>
+            <v>0.13036200000000001</v>
           </cell>
           <cell r="E147">
-            <v>410</v>
+            <v>414</v>
           </cell>
         </row>
         <row r="148">
           <cell r="D148">
-            <v>0.130574</v>
+            <v>0.13029499999999999</v>
           </cell>
           <cell r="E148">
-            <v>411</v>
+            <v>415</v>
           </cell>
         </row>
         <row r="149">
           <cell r="D149">
-            <v>0.13050200000000001</v>
+            <v>0.130163</v>
           </cell>
           <cell r="E149">
-            <v>412</v>
+            <v>417</v>
           </cell>
         </row>
         <row r="150">
           <cell r="D150">
-            <v>0.13036200000000001</v>
+            <v>0.13009999999999999</v>
           </cell>
           <cell r="E150">
-            <v>414</v>
+            <v>418</v>
           </cell>
         </row>
         <row r="151">
           <cell r="D151">
-            <v>0.13029499999999999</v>
+            <v>0.13003799999999999</v>
           </cell>
           <cell r="E151">
-            <v>415</v>
+            <v>419</v>
           </cell>
         </row>
         <row r="152">
           <cell r="D152">
-            <v>0.130163</v>
+            <v>0.12991900000000001</v>
           </cell>
           <cell r="E152">
-            <v>417</v>
+            <v>421</v>
           </cell>
         </row>
         <row r="153">
           <cell r="D153">
-            <v>0.13009999999999999</v>
+            <v>0.129861</v>
           </cell>
           <cell r="E153">
-            <v>418</v>
+            <v>422</v>
           </cell>
         </row>
         <row r="154">
           <cell r="D154">
-            <v>0.13003799999999999</v>
+            <v>0.129805</v>
           </cell>
           <cell r="E154">
-            <v>419</v>
+            <v>423</v>
           </cell>
         </row>
         <row r="155">
           <cell r="D155">
-            <v>0.12991900000000001</v>
+            <v>0.12975100000000001</v>
           </cell>
           <cell r="E155">
-            <v>421</v>
+            <v>424</v>
           </cell>
         </row>
         <row r="156">
           <cell r="D156">
-            <v>0.129861</v>
+            <v>0.12969800000000001</v>
           </cell>
           <cell r="E156">
-            <v>422</v>
+            <v>425</v>
           </cell>
         </row>
         <row r="157">
           <cell r="D157">
-            <v>0.129805</v>
+            <v>0.12964600000000001</v>
           </cell>
           <cell r="E157">
-            <v>423</v>
+            <v>426</v>
           </cell>
         </row>
         <row r="158">
           <cell r="D158">
-            <v>0.12975100000000001</v>
+            <v>0.12959599999999999</v>
           </cell>
           <cell r="E158">
-            <v>424</v>
+            <v>427</v>
           </cell>
         </row>
         <row r="159">
           <cell r="D159">
-            <v>0.12969800000000001</v>
+            <v>0.129547</v>
           </cell>
           <cell r="E159">
-            <v>425</v>
+            <v>428</v>
           </cell>
         </row>
         <row r="160">
           <cell r="D160">
-            <v>0.12964600000000001</v>
+            <v>0.1295</v>
           </cell>
           <cell r="E160">
-            <v>426</v>
+            <v>429</v>
           </cell>
         </row>
         <row r="161">
           <cell r="D161">
-            <v>0.12959599999999999</v>
+            <v>0.12945499999999999</v>
           </cell>
           <cell r="E161">
-            <v>427</v>
+            <v>430</v>
           </cell>
         </row>
         <row r="162">
           <cell r="D162">
-            <v>0.129547</v>
+            <v>0.129411</v>
           </cell>
           <cell r="E162">
-            <v>428</v>
+            <v>431</v>
           </cell>
         </row>
         <row r="163">
           <cell r="D163">
-            <v>0.1295</v>
+            <v>0.12928799999999999</v>
           </cell>
           <cell r="E163">
-            <v>429</v>
+            <v>434</v>
           </cell>
         </row>
         <row r="164">
           <cell r="D164">
-            <v>0.12945499999999999</v>
+            <v>0.12925</v>
           </cell>
           <cell r="E164">
-            <v>430</v>
+            <v>435</v>
           </cell>
         </row>
         <row r="165">
           <cell r="D165">
-            <v>0.129411</v>
+            <v>0.12917899999999999</v>
           </cell>
           <cell r="E165">
-            <v>431</v>
+            <v>437</v>
           </cell>
         </row>
         <row r="166">
           <cell r="D166">
-            <v>0.12928799999999999</v>
+            <v>0.12911400000000001</v>
           </cell>
           <cell r="E166">
-            <v>434</v>
+            <v>439</v>
           </cell>
         </row>
         <row r="167">
           <cell r="D167">
-            <v>0.12925</v>
+            <v>0.129084</v>
           </cell>
           <cell r="E167">
-            <v>435</v>
+            <v>440</v>
           </cell>
         </row>
         <row r="168">
           <cell r="D168">
-            <v>0.12917899999999999</v>
+            <v>0.129056</v>
           </cell>
           <cell r="E168">
-            <v>437</v>
+            <v>441</v>
           </cell>
         </row>
         <row r="169">
           <cell r="D169">
-            <v>0.12911400000000001</v>
+            <v>0.129029</v>
           </cell>
           <cell r="E169">
-            <v>439</v>
+            <v>442</v>
           </cell>
         </row>
         <row r="170">
           <cell r="D170">
-            <v>0.129084</v>
+            <v>0.12900300000000001</v>
           </cell>
           <cell r="E170">
-            <v>440</v>
+            <v>443</v>
           </cell>
         </row>
         <row r="171">
           <cell r="D171">
-            <v>0.129056</v>
+            <v>0.12898000000000001</v>
           </cell>
           <cell r="E171">
-            <v>441</v>
+            <v>444</v>
           </cell>
         </row>
         <row r="172">
           <cell r="D172">
-            <v>0.129029</v>
+            <v>0.12895799999999999</v>
           </cell>
           <cell r="E172">
-            <v>442</v>
+            <v>445</v>
           </cell>
         </row>
         <row r="173">
           <cell r="D173">
-            <v>0.12900300000000001</v>
+            <v>0.128937</v>
           </cell>
           <cell r="E173">
-            <v>443</v>
+            <v>446</v>
           </cell>
         </row>
         <row r="174">
           <cell r="D174">
-            <v>0.12898000000000001</v>
+            <v>0.128918</v>
           </cell>
           <cell r="E174">
-            <v>444</v>
+            <v>447</v>
           </cell>
         </row>
         <row r="175">
           <cell r="D175">
-            <v>0.12895799999999999</v>
+            <v>0.12890099999999999</v>
           </cell>
           <cell r="E175">
-            <v>445</v>
+            <v>448</v>
           </cell>
         </row>
         <row r="176">
           <cell r="D176">
-            <v>0.128937</v>
+            <v>0.128885</v>
           </cell>
           <cell r="E176">
-            <v>446</v>
+            <v>449</v>
           </cell>
         </row>
         <row r="177">
           <cell r="D177">
-            <v>0.128918</v>
+            <v>0.12887100000000001</v>
           </cell>
           <cell r="E177">
-            <v>447</v>
+            <v>450</v>
           </cell>
         </row>
         <row r="178">
           <cell r="D178">
-            <v>0.12890099999999999</v>
+            <v>0.12883900000000001</v>
           </cell>
           <cell r="E178">
-            <v>448</v>
+            <v>453</v>
           </cell>
         </row>
         <row r="179">
           <cell r="D179">
-            <v>0.128885</v>
+            <v>0.128831</v>
           </cell>
           <cell r="E179">
-            <v>449</v>
+            <v>454</v>
           </cell>
         </row>
         <row r="180">
           <cell r="D180">
-            <v>0.12887100000000001</v>
+            <v>0.128825</v>
           </cell>
           <cell r="E180">
-            <v>450</v>
+            <v>455</v>
           </cell>
         </row>
         <row r="181">
           <cell r="D181">
-            <v>0.12883900000000001</v>
+            <v>0.12881899999999999</v>
           </cell>
           <cell r="E181">
-            <v>453</v>
+            <v>457</v>
           </cell>
         </row>
         <row r="182">
           <cell r="D182">
-            <v>0.128831</v>
+            <v>0.12881799999999999</v>
           </cell>
           <cell r="E182">
-            <v>454</v>
+            <v>458</v>
           </cell>
         </row>
         <row r="183">
           <cell r="D183">
-            <v>0.128825</v>
+            <v>0.12881799999999999</v>
           </cell>
           <cell r="E183">
-            <v>455</v>
+            <v>459</v>
           </cell>
         </row>
         <row r="184">
           <cell r="D184">
-            <v>0.12881899999999999</v>
+            <v>0.12882099999999999</v>
           </cell>
           <cell r="E184">
-            <v>457</v>
+            <v>460</v>
           </cell>
         </row>
         <row r="185">
           <cell r="D185">
-            <v>0.12881799999999999</v>
+            <v>0.128825</v>
           </cell>
           <cell r="E185">
-            <v>458</v>
+            <v>461</v>
           </cell>
         </row>
         <row r="186">
           <cell r="D186">
-            <v>0.12881799999999999</v>
+            <v>0.128831</v>
           </cell>
           <cell r="E186">
-            <v>459</v>
+            <v>462</v>
           </cell>
         </row>
         <row r="187">
           <cell r="D187">
-            <v>0.12882099999999999</v>
+            <v>0.12884799999999999</v>
           </cell>
           <cell r="E187">
-            <v>460</v>
+            <v>464</v>
           </cell>
         </row>
         <row r="188">
           <cell r="D188">
-            <v>0.128825</v>
+            <v>0.128859</v>
           </cell>
           <cell r="E188">
-            <v>461</v>
+            <v>465</v>
           </cell>
         </row>
         <row r="189">
           <cell r="D189">
-            <v>0.128831</v>
+            <v>0.128886</v>
           </cell>
           <cell r="E189">
-            <v>462</v>
+            <v>467</v>
           </cell>
         </row>
         <row r="190">
           <cell r="D190">
-            <v>0.12884799999999999</v>
+            <v>0.12890199999999999</v>
           </cell>
           <cell r="E190">
-            <v>464</v>
+            <v>468</v>
           </cell>
         </row>
         <row r="191">
           <cell r="D191">
-            <v>0.128859</v>
+            <v>0.128939</v>
           </cell>
           <cell r="E191">
-            <v>465</v>
+            <v>470</v>
           </cell>
         </row>
         <row r="192">
           <cell r="D192">
-            <v>0.128886</v>
+            <v>0.12896099999999999</v>
           </cell>
           <cell r="E192">
-            <v>467</v>
+            <v>471</v>
           </cell>
         </row>
         <row r="193">
           <cell r="D193">
-            <v>0.12890199999999999</v>
+            <v>0.12898399999999999</v>
           </cell>
           <cell r="E193">
-            <v>468</v>
+            <v>472</v>
           </cell>
         </row>
         <row r="194">
           <cell r="D194">
-            <v>0.128939</v>
+            <v>0.12900800000000001</v>
           </cell>
           <cell r="E194">
-            <v>470</v>
+            <v>473</v>
           </cell>
         </row>
         <row r="195">
           <cell r="D195">
-            <v>0.12896099999999999</v>
+            <v>0.12903500000000001</v>
           </cell>
           <cell r="E195">
-            <v>471</v>
+            <v>474</v>
           </cell>
         </row>
         <row r="196">
           <cell r="D196">
-            <v>0.12898399999999999</v>
+            <v>0.12906300000000001</v>
           </cell>
           <cell r="E196">
-            <v>472</v>
+            <v>475</v>
           </cell>
         </row>
         <row r="197">
           <cell r="D197">
-            <v>0.12900800000000001</v>
+            <v>0.12909300000000001</v>
           </cell>
           <cell r="E197">
-            <v>473</v>
+            <v>476</v>
           </cell>
         </row>
         <row r="198">
           <cell r="D198">
-            <v>0.12903500000000001</v>
+            <v>0.12912499999999999</v>
           </cell>
           <cell r="E198">
-            <v>474</v>
+            <v>477</v>
           </cell>
         </row>
         <row r="199">
           <cell r="D199">
-            <v>0.12906300000000001</v>
+            <v>0.129159</v>
           </cell>
           <cell r="E199">
-            <v>475</v>
+            <v>478</v>
           </cell>
         </row>
         <row r="200">
           <cell r="D200">
-            <v>0.12909300000000001</v>
+            <v>0.129194</v>
           </cell>
           <cell r="E200">
-            <v>476</v>
+            <v>479</v>
           </cell>
         </row>
         <row r="201">
           <cell r="D201">
-            <v>0.12912499999999999</v>
+            <v>0.12927</v>
           </cell>
           <cell r="E201">
-            <v>477</v>
+            <v>481</v>
           </cell>
         </row>
         <row r="202">
           <cell r="D202">
-            <v>0.129159</v>
+            <v>0.129354</v>
           </cell>
           <cell r="E202">
-            <v>478</v>
+            <v>483</v>
           </cell>
         </row>
         <row r="203">
           <cell r="D203">
-            <v>0.129194</v>
+            <v>0.12939800000000001</v>
           </cell>
           <cell r="E203">
-            <v>479</v>
+            <v>484</v>
           </cell>
         </row>
         <row r="204">
           <cell r="D204">
-            <v>0.12927</v>
+            <v>0.129444</v>
           </cell>
           <cell r="E204">
-            <v>481</v>
+            <v>485</v>
           </cell>
         </row>
         <row r="205">
           <cell r="D205">
-            <v>0.129354</v>
+            <v>0.129492</v>
           </cell>
           <cell r="E205">
-            <v>483</v>
+            <v>486</v>
           </cell>
         </row>
         <row r="206">
           <cell r="D206">
-            <v>0.12939800000000001</v>
+            <v>0.12954199999999999</v>
           </cell>
           <cell r="E206">
-            <v>484</v>
+            <v>487</v>
           </cell>
         </row>
         <row r="207">
           <cell r="D207">
-            <v>0.129444</v>
+            <v>0.12959399999999999</v>
           </cell>
           <cell r="E207">
-            <v>485</v>
+            <v>488</v>
           </cell>
         </row>
         <row r="208">
           <cell r="D208">
-            <v>0.129492</v>
+            <v>0.12964700000000001</v>
           </cell>
           <cell r="E208">
-            <v>486</v>
+            <v>489</v>
           </cell>
         </row>
         <row r="209">
           <cell r="D209">
-            <v>0.12954199999999999</v>
+            <v>0.12970300000000001</v>
           </cell>
           <cell r="E209">
-            <v>487</v>
+            <v>490</v>
           </cell>
         </row>
         <row r="210">
           <cell r="D210">
-            <v>0.12959399999999999</v>
+            <v>0.12975999999999999</v>
           </cell>
           <cell r="E210">
-            <v>488</v>
+            <v>491</v>
           </cell>
         </row>
         <row r="211">
           <cell r="D211">
-            <v>0.12964700000000001</v>
+            <v>0.12988</v>
           </cell>
           <cell r="E211">
-            <v>489</v>
+            <v>493</v>
           </cell>
         </row>
         <row r="212">
           <cell r="D212">
-            <v>0.12970300000000001</v>
+            <v>0.129942</v>
           </cell>
           <cell r="E212">
-            <v>490</v>
+            <v>494</v>
           </cell>
         </row>
         <row r="213">
           <cell r="D213">
-            <v>0.12975999999999999</v>
+            <v>0.13000700000000001</v>
           </cell>
           <cell r="E213">
-            <v>491</v>
+            <v>495</v>
           </cell>
         </row>
         <row r="214">
           <cell r="D214">
-            <v>0.12988</v>
+            <v>0.130074</v>
           </cell>
           <cell r="E214">
-            <v>493</v>
+            <v>496</v>
           </cell>
         </row>
         <row r="215">
           <cell r="D215">
-            <v>0.129942</v>
+            <v>0.13014200000000001</v>
           </cell>
           <cell r="E215">
-            <v>494</v>
+            <v>497</v>
           </cell>
         </row>
         <row r="216">
           <cell r="D216">
-            <v>0.13000700000000001</v>
+            <v>0.13021199999999999</v>
           </cell>
           <cell r="E216">
-            <v>495</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="D217">
-            <v>0.130074</v>
-          </cell>
-          <cell r="E217">
-            <v>496</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="D218">
-            <v>0.13014200000000001</v>
-          </cell>
-          <cell r="E218">
-            <v>497</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="D219">
-            <v>0.13021199999999999</v>
-          </cell>
-          <cell r="E219">
             <v>498</v>
           </cell>
         </row>
@@ -36739,7 +36733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -36755,7 +36749,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36770,7 +36764,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36784,8 +36778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7B53C2-337D-48F7-A143-34AF6240A5F5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>